<commit_message>
Project 4 Multiplatform report
</commit_message>
<xml_diff>
--- a/Proyectos/Proyecto4 - Finanzas personales multidispositivos/Finanzas.xlsx
+++ b/Proyectos/Proyecto4 - Finanzas personales multidispositivos/Finanzas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\Computacion\Data\Analytics\Udemy\Power BI\Curso Power BI – Análisis de Datos y Business Intelligence\Proyectos\Proyecto4 - Finanzas personales multidispositivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE8B5132-215A-4EE1-AB2F-861271B70599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513433F5-56EF-4D8A-BA30-ECE2654E7EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos" sheetId="11" r:id="rId1"/>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -284,17 +284,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -574,6 +576,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4292D75-D3CE-43DB-8E76-57A0D5FF7976}" name="TablaIngresos" displayName="TablaIngresos" ref="A3:C51" totalsRowShown="0">
+  <autoFilter ref="A3:C51" xr:uid="{E4292D75-D3CE-43DB-8E76-57A0D5FF7976}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{408B86FB-74D6-4B2D-94C0-753A1E55393A}" name="Categoria"/>
+    <tableColumn id="2" xr3:uid="{366D0BBA-42A0-4955-8BA6-0A0B22444115}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{BE23A87A-F0FC-4ED7-BF4F-44D0BC452D31}" name="Cantidad"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaGastos" displayName="TablaGastos" ref="A3:C219" totalsRowShown="0">
   <autoFilter ref="A3:C219" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C217">
@@ -581,14 +595,14 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categoria"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cantidad"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TablaMetas" displayName="TablaMetas" ref="A3:C27" totalsRowShown="0">
   <autoFilter ref="A3:C27" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
@@ -600,8 +614,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TablaPresupuesto" displayName="TablaPresupuesto" ref="A3:Y12" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TablaPresupuesto" displayName="TablaPresupuesto" ref="A3:Y12" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:Y12" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -925,11 +939,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="3" customWidth="1"/>
@@ -985,52 +999,43 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="3">
         <v>45992</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10078</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4">
-        <v>10078</v>
-      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="3">
         <v>45992</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>13888</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5">
-        <v>13888</v>
-      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="3">
         <v>45962</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>10002</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6">
-        <v>10002</v>
-      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="3">
         <v>45962</v>
       </c>
       <c r="C7">
@@ -1042,7 +1047,7 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="3">
         <v>45931</v>
       </c>
       <c r="C8">
@@ -1054,7 +1059,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="3">
         <v>45931</v>
       </c>
       <c r="C9">
@@ -1066,7 +1071,7 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="3">
         <v>45901</v>
       </c>
       <c r="C10">
@@ -1078,7 +1083,7 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="3">
         <v>45901</v>
       </c>
       <c r="C11">
@@ -1090,7 +1095,7 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="3">
         <v>45870</v>
       </c>
       <c r="C12">
@@ -1102,7 +1107,7 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="3">
         <v>45870</v>
       </c>
       <c r="C13">
@@ -1114,7 +1119,7 @@
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="3">
         <v>45839</v>
       </c>
       <c r="C14">
@@ -1126,7 +1131,7 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="3">
         <v>45839</v>
       </c>
       <c r="C15">
@@ -1138,7 +1143,7 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="3">
         <v>45809</v>
       </c>
       <c r="C16">
@@ -1150,7 +1155,7 @@
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="3">
         <v>45809</v>
       </c>
       <c r="C17">
@@ -1162,7 +1167,7 @@
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="3">
         <v>45778</v>
       </c>
       <c r="C18">
@@ -1174,7 +1179,7 @@
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="3">
         <v>45778</v>
       </c>
       <c r="C19">
@@ -1186,7 +1191,7 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="3">
         <v>45748</v>
       </c>
       <c r="C20">
@@ -1198,7 +1203,7 @@
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="3">
         <v>45748</v>
       </c>
       <c r="C21">
@@ -1210,7 +1215,7 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="3">
         <v>45717</v>
       </c>
       <c r="C22">
@@ -1222,7 +1227,7 @@
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="3">
         <v>45717</v>
       </c>
       <c r="C23">
@@ -1234,7 +1239,7 @@
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="3">
         <v>45689</v>
       </c>
       <c r="C24">
@@ -1246,7 +1251,7 @@
       <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="3">
         <v>45689</v>
       </c>
       <c r="C25">
@@ -1258,7 +1263,7 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="3">
         <v>45658</v>
       </c>
       <c r="C26">
@@ -1270,7 +1275,7 @@
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="3">
         <v>45658</v>
       </c>
       <c r="C27">
@@ -1282,7 +1287,7 @@
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="3">
         <v>45627</v>
       </c>
       <c r="C28">
@@ -1294,7 +1299,7 @@
       <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="3">
         <v>45627</v>
       </c>
       <c r="C29">
@@ -1306,7 +1311,7 @@
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="3">
         <v>45597</v>
       </c>
       <c r="C30">
@@ -1318,7 +1323,7 @@
       <c r="A31" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="3">
         <v>45597</v>
       </c>
       <c r="C31">
@@ -1330,7 +1335,7 @@
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="3">
         <v>45566</v>
       </c>
       <c r="C32">
@@ -1342,7 +1347,7 @@
       <c r="A33" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="3">
         <v>45566</v>
       </c>
       <c r="C33">
@@ -1354,7 +1359,7 @@
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="3">
         <v>45536</v>
       </c>
       <c r="C34">
@@ -1366,7 +1371,7 @@
       <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="3">
         <v>45536</v>
       </c>
       <c r="C35">
@@ -1378,7 +1383,7 @@
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="3">
         <v>45505</v>
       </c>
       <c r="C36">
@@ -1390,7 +1395,7 @@
       <c r="A37" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="3">
         <v>45505</v>
       </c>
       <c r="C37">
@@ -1402,7 +1407,7 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="3">
         <v>45474</v>
       </c>
       <c r="C38">
@@ -1414,7 +1419,7 @@
       <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="3">
         <v>45474</v>
       </c>
       <c r="C39">
@@ -1426,7 +1431,7 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="3">
         <v>45444</v>
       </c>
       <c r="C40">
@@ -1438,7 +1443,7 @@
       <c r="A41" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="3">
         <v>45444</v>
       </c>
       <c r="C41">
@@ -1450,7 +1455,7 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="3">
         <v>45413</v>
       </c>
       <c r="C42">
@@ -1462,7 +1467,7 @@
       <c r="A43" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="3">
         <v>45413</v>
       </c>
       <c r="C43">
@@ -1474,7 +1479,7 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="3">
         <v>45383</v>
       </c>
       <c r="C44">
@@ -1486,7 +1491,7 @@
       <c r="A45" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="3">
         <v>45383</v>
       </c>
       <c r="C45">
@@ -1498,7 +1503,7 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="3">
         <v>45352</v>
       </c>
       <c r="C46">
@@ -1510,7 +1515,7 @@
       <c r="A47" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="3">
         <v>45352</v>
       </c>
       <c r="C47">
@@ -1522,7 +1527,7 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="3">
         <v>45323</v>
       </c>
       <c r="C48">
@@ -1534,7 +1539,7 @@
       <c r="A49" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="3">
         <v>45323</v>
       </c>
       <c r="C49">
@@ -1546,7 +1551,7 @@
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="3">
         <v>45292</v>
       </c>
       <c r="C50">
@@ -1558,7 +1563,7 @@
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="3">
         <v>45292</v>
       </c>
       <c r="C51">
@@ -1573,6 +1578,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1581,10 +1589,10 @@
   <dimension ref="A1:Y219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
@@ -4028,10 +4036,10 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
@@ -4367,11 +4375,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="25" width="6.109375" customWidth="1"/>

</xml_diff>